<commit_message>
add americas day 1 showflow
</commit_message>
<xml_diff>
--- a/infra-apps/infra-apps-Track-Showflow.xlsx
+++ b/infra-apps/infra-apps-Track-Showflow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\Dropbox (Personal)\GitHub\cloud-core-2020-fix2\infra-apps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanPatrick\DB\Dropbox (Personal)\GitHub\cloud-core-2020-fix2\infra-apps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005C8048-B2D6-4514-A59A-A9F8CDE7FDE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C72C14-47D8-479C-9EC3-B2A6D1A02CFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0B725299-4060-418E-A1A8-086098773DCE}"/>
+    <workbookView minimized="1" xWindow="39015" yWindow="225" windowWidth="10365" windowHeight="15570" activeTab="2" xr2:uid="{0B725299-4060-418E-A1A8-086098773DCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 2" sheetId="2" r:id="rId1"/>
@@ -476,6 +476,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -486,9 +489,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -843,24 +843,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -896,10 +896,10 @@
       <c r="K2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="40"/>
+      <c r="M2" s="41"/>
       <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
@@ -911,10 +911,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -929,10 +929,10 @@
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="1:16" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
@@ -947,10 +947,10 @@
       <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
@@ -965,10 +965,10 @@
       <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:16" s="10" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
@@ -983,10 +983,10 @@
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
@@ -1001,10 +1001,10 @@
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
@@ -1019,10 +1019,10 @@
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
@@ -1037,10 +1037,10 @@
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
@@ -1055,10 +1055,10 @@
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
@@ -1073,10 +1073,10 @@
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
@@ -1091,10 +1091,10 @@
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="9"/>
@@ -1109,10 +1109,10 @@
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="7"/>
       <c r="F14" s="13"/>
       <c r="G14" s="9"/>
@@ -1127,10 +1127,10 @@
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="7"/>
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
@@ -1145,10 +1145,10 @@
       <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="7"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
@@ -1187,14 +1187,14 @@
         <v>1</v>
       </c>
       <c r="B18" s="6">
-        <f>MOD(E18-(7/24),1)</f>
+        <f t="shared" ref="B18:B24" si="0">MOD(E18-(7/24),1)</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="38">
         <f>MOD(E18-(6/24),1)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="38">
         <f>MOD(E18-(4/24),1)</f>
         <v>0.14583333333333334</v>
       </c>
@@ -1222,15 +1222,15 @@
         <v>2</v>
       </c>
       <c r="B19" s="6">
-        <f>MOD(E19-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="C19" s="42">
-        <f t="shared" ref="C19:C24" si="0">MOD(E19-(6/24),1)</f>
+      <c r="C19" s="38">
+        <f t="shared" ref="C19:C24" si="1">MOD(E19-(6/24),1)</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="D19" s="42">
-        <f t="shared" ref="D19:D24" si="1">MOD(E19-(4/24),1)</f>
+      <c r="D19" s="38">
+        <f t="shared" ref="D19:D24" si="2">MOD(E19-(4/24),1)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="E19" s="23">
@@ -1257,15 +1257,15 @@
         <v>3</v>
       </c>
       <c r="B20" s="6">
-        <f>MOD(E20-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.14583333333333331</v>
       </c>
-      <c r="C20" s="42">
-        <f t="shared" si="0"/>
+      <c r="C20" s="38">
+        <f t="shared" si="1"/>
         <v>0.1875</v>
       </c>
-      <c r="D20" s="42">
-        <f t="shared" si="1"/>
+      <c r="D20" s="38">
+        <f t="shared" si="2"/>
         <v>0.27083333333333337</v>
       </c>
       <c r="E20" s="23">
@@ -1294,15 +1294,15 @@
         <v>4</v>
       </c>
       <c r="B21" s="6">
-        <f>MOD(E21-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.14930555555555558</v>
       </c>
-      <c r="C21" s="42">
-        <f t="shared" si="0"/>
+      <c r="C21" s="38">
+        <f t="shared" si="1"/>
         <v>0.19097222222222227</v>
       </c>
-      <c r="D21" s="42">
-        <f t="shared" si="1"/>
+      <c r="D21" s="38">
+        <f t="shared" si="2"/>
         <v>0.27430555555555558</v>
       </c>
       <c r="E21" s="23">
@@ -1329,15 +1329,15 @@
         <v>5</v>
       </c>
       <c r="B22" s="6">
-        <f>MOD(E22-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="C22" s="42">
-        <f t="shared" si="0"/>
+      <c r="C22" s="38">
+        <f t="shared" si="1"/>
         <v>0.20833333333333331</v>
       </c>
-      <c r="D22" s="42">
-        <f t="shared" si="1"/>
+      <c r="D22" s="38">
+        <f t="shared" si="2"/>
         <v>0.29166666666666663</v>
       </c>
       <c r="E22" s="23">
@@ -1364,15 +1364,15 @@
         <v>7</v>
       </c>
       <c r="B23" s="6">
-        <f>MOD(E23-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.20833333333333331</v>
       </c>
-      <c r="C23" s="42">
-        <f t="shared" si="0"/>
+      <c r="C23" s="38">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="D23" s="42">
-        <f t="shared" si="1"/>
+      <c r="D23" s="38">
+        <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
       <c r="E23" s="23">
@@ -1399,15 +1399,15 @@
         <v>8</v>
       </c>
       <c r="B24" s="6">
-        <f>MOD(E24-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.29166666666666669</v>
       </c>
-      <c r="C24" s="42">
-        <f t="shared" si="0"/>
+      <c r="C24" s="38">
+        <f t="shared" si="1"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="D24" s="42">
-        <f t="shared" si="1"/>
+      <c r="D24" s="38">
+        <f t="shared" si="2"/>
         <v>0.41666666666666674</v>
       </c>
       <c r="E24" s="23">
@@ -2271,24 +2271,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2324,10 +2324,10 @@
       <c r="K2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="40"/>
+      <c r="M2" s="41"/>
       <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2339,10 +2339,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -2357,10 +2357,10 @@
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="1:16" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
@@ -2375,10 +2375,10 @@
       <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
@@ -2393,10 +2393,10 @@
       <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:16" s="10" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
@@ -2411,10 +2411,10 @@
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
@@ -2429,10 +2429,10 @@
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
@@ -2447,10 +2447,10 @@
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
@@ -2465,10 +2465,10 @@
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
@@ -2483,10 +2483,10 @@
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
@@ -2501,10 +2501,10 @@
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
@@ -2519,10 +2519,10 @@
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="9"/>
@@ -2537,10 +2537,10 @@
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="7"/>
       <c r="F14" s="13"/>
       <c r="G14" s="9"/>
@@ -2555,10 +2555,10 @@
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="7"/>
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
@@ -2573,10 +2573,10 @@
       <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="7"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
@@ -2615,14 +2615,14 @@
         <v>1</v>
       </c>
       <c r="B18" s="6">
-        <f>MOD(E18-(7/24),1)</f>
+        <f t="shared" ref="B18:B26" si="0">MOD(E18-(7/24),1)</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="38">
         <f>MOD(E18-(6/24),1)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="38">
         <f>MOD(E18-(4/24),1)</f>
         <v>0.14583333333333334</v>
       </c>
@@ -2650,15 +2650,15 @@
         <v>2</v>
       </c>
       <c r="B19" s="6">
-        <f>MOD(E19-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="C19" s="42">
-        <f t="shared" ref="C19:C26" si="0">MOD(E19-(6/24),1)</f>
+      <c r="C19" s="38">
+        <f t="shared" ref="C19:C26" si="1">MOD(E19-(6/24),1)</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="D19" s="42">
-        <f t="shared" ref="D19:D26" si="1">MOD(E19-(4/24),1)</f>
+      <c r="D19" s="38">
+        <f t="shared" ref="D19:D26" si="2">MOD(E19-(4/24),1)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="E19" s="23">
@@ -2685,15 +2685,15 @@
         <v>3</v>
       </c>
       <c r="B20" s="6">
-        <f>MOD(E20-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>5.2083333333333315E-2</v>
       </c>
-      <c r="C20" s="42">
-        <f t="shared" si="0"/>
+      <c r="C20" s="38">
+        <f t="shared" si="1"/>
         <v>9.375E-2</v>
       </c>
-      <c r="D20" s="42">
-        <f t="shared" si="1"/>
+      <c r="D20" s="38">
+        <f t="shared" si="2"/>
         <v>0.17708333333333334</v>
       </c>
       <c r="E20" s="23">
@@ -2724,15 +2724,15 @@
         <v>4</v>
       </c>
       <c r="B21" s="6">
-        <f>MOD(E21-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="C21" s="42">
-        <f t="shared" si="0"/>
+      <c r="C21" s="38">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="D21" s="42">
-        <f t="shared" si="1"/>
+      <c r="D21" s="38">
+        <f t="shared" si="2"/>
         <v>0.20833333333333334</v>
       </c>
       <c r="E21" s="23">
@@ -2755,15 +2755,15 @@
     <row r="22" spans="1:16" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="6">
-        <f>MOD(E22-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.10416666666666663</v>
       </c>
-      <c r="C22" s="42">
-        <f t="shared" si="0"/>
+      <c r="C22" s="38">
+        <f t="shared" si="1"/>
         <v>0.14583333333333331</v>
       </c>
-      <c r="D22" s="42">
-        <f t="shared" si="1"/>
+      <c r="D22" s="38">
+        <f t="shared" si="2"/>
         <v>0.22916666666666666</v>
       </c>
       <c r="E22" s="23">
@@ -2786,15 +2786,15 @@
     <row r="23" spans="1:16" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="6">
-        <f>MOD(E23-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.11458333333333331</v>
       </c>
-      <c r="C23" s="42">
-        <f t="shared" si="0"/>
+      <c r="C23" s="38">
+        <f t="shared" si="1"/>
         <v>0.15625</v>
       </c>
-      <c r="D23" s="42">
-        <f t="shared" si="1"/>
+      <c r="D23" s="38">
+        <f t="shared" si="2"/>
         <v>0.23958333333333334</v>
       </c>
       <c r="E23" s="23">
@@ -2819,15 +2819,15 @@
         <v>5</v>
       </c>
       <c r="B24" s="6">
-        <f>MOD(E24-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="C24" s="42">
-        <f t="shared" si="0"/>
+      <c r="C24" s="38">
+        <f t="shared" si="1"/>
         <v>0.20833333333333331</v>
       </c>
-      <c r="D24" s="42">
-        <f t="shared" si="1"/>
+      <c r="D24" s="38">
+        <f t="shared" si="2"/>
         <v>0.29166666666666663</v>
       </c>
       <c r="E24" s="23">
@@ -2854,15 +2854,15 @@
         <v>7</v>
       </c>
       <c r="B25" s="6">
-        <f>MOD(E25-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.20833333333333331</v>
       </c>
-      <c r="C25" s="42">
-        <f t="shared" si="0"/>
+      <c r="C25" s="38">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="D25" s="42">
-        <f t="shared" si="1"/>
+      <c r="D25" s="38">
+        <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
       <c r="E25" s="23">
@@ -2889,15 +2889,15 @@
         <v>8</v>
       </c>
       <c r="B26" s="6">
-        <f>MOD(E26-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.29166666666666669</v>
       </c>
-      <c r="C26" s="42">
-        <f t="shared" si="0"/>
+      <c r="C26" s="38">
+        <f t="shared" si="1"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="D26" s="42">
-        <f t="shared" si="1"/>
+      <c r="D26" s="38">
+        <f t="shared" si="2"/>
         <v>0.41666666666666674</v>
       </c>
       <c r="E26" s="23">
@@ -3738,16 +3738,17 @@
   <dimension ref="A1:P66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="33" customWidth="1"/>
-    <col min="2" max="5" width="10.5703125" style="34" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" style="34" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" style="34" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="35" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="40.42578125" style="36" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="36" customWidth="1"/>
@@ -3763,24 +3764,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
     </row>
     <row r="2" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3816,10 +3817,10 @@
       <c r="K2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="40"/>
+      <c r="M2" s="41"/>
       <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
@@ -3831,10 +3832,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -3849,10 +3850,10 @@
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="1:16" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
@@ -3867,10 +3868,10 @@
       <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
@@ -3885,10 +3886,10 @@
       <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:16" s="10" customFormat="1" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="6"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
@@ -3903,10 +3904,10 @@
       <c r="P6" s="12"/>
     </row>
     <row r="7" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
       <c r="G7" s="9"/>
@@ -3921,10 +3922,10 @@
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
@@ -3939,10 +3940,10 @@
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
@@ -3957,10 +3958,10 @@
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="7"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
@@ -3975,10 +3976,10 @@
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="7"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
@@ -3993,10 +3994,10 @@
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
       <c r="G12" s="9"/>
@@ -4011,10 +4012,10 @@
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="7"/>
       <c r="F13" s="13"/>
       <c r="G13" s="9"/>
@@ -4029,10 +4030,10 @@
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="7"/>
       <c r="F14" s="13"/>
       <c r="G14" s="9"/>
@@ -4047,10 +4048,10 @@
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="7"/>
       <c r="F15" s="13"/>
       <c r="G15" s="9"/>
@@ -4065,10 +4066,10 @@
       <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="7"/>
       <c r="F16" s="13"/>
       <c r="G16" s="9"/>
@@ -4107,14 +4108,14 @@
         <v>1</v>
       </c>
       <c r="B18" s="6">
-        <f>MOD(E18-(7/24),1)</f>
+        <f t="shared" ref="B18:B26" si="0">MOD(E18-(7/24),1)</f>
         <v>2.0833333333333315E-2</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="38">
         <f>MOD(E18-(6/24),1)</f>
         <v>6.25E-2</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="38">
         <f>MOD(E18-(4/24),1)</f>
         <v>0.14583333333333334</v>
       </c>
@@ -4142,15 +4143,15 @@
         <v>2</v>
       </c>
       <c r="B19" s="6">
-        <f>MOD(E19-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="C19" s="42">
-        <f t="shared" ref="C19:C26" si="0">MOD(E19-(6/24),1)</f>
+      <c r="C19" s="38">
+        <f t="shared" ref="C19:C26" si="1">MOD(E19-(6/24),1)</f>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="D19" s="42">
-        <f t="shared" ref="D19:D26" si="1">MOD(E19-(4/24),1)</f>
+      <c r="D19" s="38">
+        <f t="shared" ref="D19:D26" si="2">MOD(E19-(4/24),1)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="E19" s="23">
@@ -4177,15 +4178,15 @@
         <v>3</v>
       </c>
       <c r="B20" s="6">
-        <f>MOD(E20-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="C20" s="42">
-        <f t="shared" si="0"/>
+      <c r="C20" s="38">
+        <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="D20" s="42">
-        <f t="shared" si="1"/>
+      <c r="D20" s="38">
+        <f t="shared" si="2"/>
         <v>0.20833333333333334</v>
       </c>
       <c r="E20" s="23">
@@ -4216,15 +4217,15 @@
         <v>4</v>
       </c>
       <c r="B21" s="6">
-        <f>MOD(E21-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>8.680555555555558E-2</v>
       </c>
-      <c r="C21" s="42">
-        <f t="shared" si="0"/>
+      <c r="C21" s="38">
+        <f t="shared" si="1"/>
         <v>0.12847222222222227</v>
       </c>
-      <c r="D21" s="42">
-        <f t="shared" si="1"/>
+      <c r="D21" s="38">
+        <f t="shared" si="2"/>
         <v>0.21180555555555561</v>
       </c>
       <c r="E21" s="23">
@@ -4251,15 +4252,15 @@
         <v>5</v>
       </c>
       <c r="B22" s="6">
-        <f>MOD(E22-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="C22" s="42">
-        <f t="shared" si="0"/>
+      <c r="C22" s="38">
+        <f t="shared" si="1"/>
         <v>0.20833333333333331</v>
       </c>
-      <c r="D22" s="42">
-        <f t="shared" si="1"/>
+      <c r="D22" s="38">
+        <f t="shared" si="2"/>
         <v>0.29166666666666663</v>
       </c>
       <c r="E22" s="23">
@@ -4284,15 +4285,15 @@
     <row r="23" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="6">
-        <f>MOD(E23-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.20833333333333331</v>
       </c>
-      <c r="C23" s="42">
-        <f t="shared" si="0"/>
+      <c r="C23" s="38">
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="D23" s="42">
-        <f t="shared" si="1"/>
+      <c r="D23" s="38">
+        <f t="shared" si="2"/>
         <v>0.33333333333333337</v>
       </c>
       <c r="E23" s="23">
@@ -4319,15 +4320,15 @@
         <v>3</v>
       </c>
       <c r="B24" s="6">
-        <f>MOD(E24-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.24999999999999994</v>
       </c>
-      <c r="C24" s="42">
-        <f t="shared" ref="C24" si="2">MOD(E24-(6/24),1)</f>
+      <c r="C24" s="38">
+        <f t="shared" ref="C24" si="3">MOD(E24-(6/24),1)</f>
         <v>0.29166666666666663</v>
       </c>
-      <c r="D24" s="42">
-        <f t="shared" si="1"/>
+      <c r="D24" s="38">
+        <f t="shared" si="2"/>
         <v>0.375</v>
       </c>
       <c r="E24" s="23">
@@ -4356,15 +4357,15 @@
         <v>7</v>
       </c>
       <c r="B25" s="6">
-        <f>MOD(E25-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.25347222222222227</v>
       </c>
-      <c r="C25" s="42">
-        <f t="shared" si="0"/>
+      <c r="C25" s="38">
+        <f t="shared" si="1"/>
         <v>0.29513888888888895</v>
       </c>
-      <c r="D25" s="42">
-        <f t="shared" si="1"/>
+      <c r="D25" s="38">
+        <f t="shared" si="2"/>
         <v>0.37847222222222232</v>
       </c>
       <c r="E25" s="23">
@@ -4393,15 +4394,15 @@
         <v>8</v>
       </c>
       <c r="B26" s="6">
-        <f>MOD(E26-(7/24),1)</f>
+        <f t="shared" si="0"/>
         <v>0.29166666666666669</v>
       </c>
-      <c r="C26" s="42">
-        <f t="shared" si="0"/>
+      <c r="C26" s="38">
+        <f t="shared" si="1"/>
         <v>0.33333333333333337</v>
       </c>
-      <c r="D26" s="42">
-        <f t="shared" si="1"/>
+      <c r="D26" s="38">
+        <f t="shared" si="2"/>
         <v>0.41666666666666674</v>
       </c>
       <c r="E26" s="23">

</xml_diff>